<commit_message>
edit command for statistics
</commit_message>
<xml_diff>
--- a/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
+++ b/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TestSimulator\Simulator\Simulator\bin\Debug\temp\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279E312E-5172-4B73-9E86-476DBA6981D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C61BDEC-3911-4470-91C3-9016E61C5778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{AF2D361D-D59F-4B5F-BBBC-F321EE7A1270}"/>
+    <workbookView xWindow="12285" yWindow="2940" windowWidth="14415" windowHeight="13260" xr2:uid="{AF2D361D-D59F-4B5F-BBBC-F321EE7A1270}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>ФИО</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>П4</t>
+  </si>
+  <si>
+    <t>fdf</t>
+  </si>
+  <si>
+    <t>dfdf</t>
+  </si>
+  <si>
+    <t>dfd</t>
   </si>
 </sst>
 </file>
@@ -456,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8F6418-E957-4301-9F50-E8E14120CAB9}">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,6 +659,26 @@
       </c>
       <c r="AE3" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add deleting old rows excel
</commit_message>
<xml_diff>
--- a/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
+++ b/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TestSimulator\Simulator\Simulator\bin\Debug\temp\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C61BDEC-3911-4470-91C3-9016E61C5778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F8161-284A-4145-8344-599D04BC1C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12285" yWindow="2940" windowWidth="14415" windowHeight="13260" xr2:uid="{AF2D361D-D59F-4B5F-BBBC-F321EE7A1270}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>ФИО</t>
   </si>
@@ -99,15 +99,6 @@
   </si>
   <si>
     <t>П4</t>
-  </si>
-  <si>
-    <t>fdf</t>
-  </si>
-  <si>
-    <t>dfdf</t>
-  </si>
-  <si>
-    <t>dfd</t>
   </si>
 </sst>
 </file>
@@ -465,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8F6418-E957-4301-9F50-E8E14120CAB9}">
-  <dimension ref="A1:AE9"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,34 +652,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="W1:AE1"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:V1"/>
@@ -699,11 +669,12 @@
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W1:AE1"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
debug parce user stats
</commit_message>
<xml_diff>
--- a/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
+++ b/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TestSimulator\Simulator\Simulator\bin\Debug\temp\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2F8161-284A-4145-8344-599D04BC1C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198DC3BA-165B-4217-9A01-FD6BA35D9B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12285" yWindow="2940" windowWidth="14415" windowHeight="13260" xr2:uid="{AF2D361D-D59F-4B5F-BBBC-F321EE7A1270}"/>
+    <workbookView xWindow="7155" yWindow="2940" windowWidth="14415" windowHeight="13260" xr2:uid="{2148F73A-ECB1-46C7-BCA4-709A0BF7AD17}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>ФИО</t>
   </si>
@@ -99,6 +99,24 @@
   </si>
   <si>
     <t>П4</t>
+  </si>
+  <si>
+    <t>Куляй Кирилл</t>
+  </si>
+  <si>
+    <t>3530404-10002</t>
+  </si>
+  <si>
+    <t>5;</t>
+  </si>
+  <si>
+    <t>1;2;3;</t>
+  </si>
+  <si>
+    <t>5;6;7;</t>
+  </si>
+  <si>
+    <t>3;4;5;</t>
   </si>
 </sst>
 </file>
@@ -134,9 +152,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -455,11 +479,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8F6418-E957-4301-9F50-E8E14120CAB9}">
-  <dimension ref="A1:AE3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A96EF44-42F4-4205-8DCA-8852AE4654C7}">
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,112 +492,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:31" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2" t="s">
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2" t="s">
+      <c r="V2" s="4"/>
+      <c r="W2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="Z2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2" t="s">
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="2"/>
+      <c r="AC2" s="4"/>
       <c r="AD2" s="1" t="s">
         <v>17</v>
       </c>
@@ -582,16 +606,16 @@
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
@@ -628,8 +652,8 @@
       <c r="V3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
       <c r="Y3" s="1" t="s">
         <v>20</v>
       </c>
@@ -650,6 +674,101 @@
       </c>
       <c r="AE3" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1729203905</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45061.469756944447</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45061.451342592591</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-3</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.121875E-4</v>
+      </c>
+      <c r="J4" s="3">
+        <v>8.5081018518518513E-5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5.6774991666666698E-2</v>
+      </c>
+      <c r="L4" s="1">
+        <v>8.5256788333333305E-2</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="O4" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="R4" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="3">
+        <v>5.4247685185185192E-5</v>
+      </c>
+      <c r="X4" s="3">
+        <v>7.0474537037037036E-5</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>8.9797336666666699E-2</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug excel case pt1
</commit_message>
<xml_diff>
--- a/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
+++ b/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TestSimulator\Simulator\Simulator\bin\Debug\temp\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B51768-C923-4758-B7C8-4A998B0412F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C7508A-0644-4BE1-B6AD-B47B23B4A079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7845" yWindow="2940" windowWidth="14415" windowHeight="13260" xr2:uid="{8E2B3CB3-AB10-496A-9F08-311CA960E8CE}"/>
+    <workbookView xWindow="13185" yWindow="765" windowWidth="16455" windowHeight="20625" xr2:uid="{8E2B3CB3-AB10-496A-9F08-311CA960E8CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
   <si>
     <t>ФИО</t>
   </si>
@@ -102,24 +102,6 @@
   </si>
   <si>
     <t>П5</t>
-  </si>
-  <si>
-    <t>Куляй Кирилл</t>
-  </si>
-  <si>
-    <t>3530404-10002</t>
-  </si>
-  <si>
-    <t>5-</t>
-  </si>
-  <si>
-    <t>1-2-3-4-5-</t>
-  </si>
-  <si>
-    <t>1-</t>
-  </si>
-  <si>
-    <t>1-2-</t>
   </si>
 </sst>
 </file>
@@ -155,18 +137,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -483,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F679A1BC-AC5E-4533-838D-9592A9E53D2B}">
-  <dimension ref="A1:AJ4"/>
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A3"/>
@@ -704,118 +680,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1729203905</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="3">
-        <v>45062.728171296294</v>
-      </c>
-      <c r="E4" s="3">
-        <v>45062.728958333333</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="1">
-        <v>8</v>
-      </c>
-      <c r="H4" s="1">
-        <v>5</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1.134837962962963E-4</v>
-      </c>
-      <c r="J4" s="4">
-        <v>9.6493055555555557E-5</v>
-      </c>
-      <c r="K4" s="1">
-        <v>6.2628884166666704E-2</v>
-      </c>
-      <c r="L4" s="1">
-        <v>8.8554540833333306E-2</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="O4" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>-1.5</v>
-      </c>
-      <c r="R4" s="1">
-        <v>-1.5</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W4" s="4">
-        <v>2.4668981481481482E-4</v>
-      </c>
-      <c r="X4" s="4">
-        <v>2.3930555555555554E-4</v>
-      </c>
-      <c r="Y4" s="1">
-        <v>6.7195554166666699E-2</v>
-      </c>
-      <c r="Z4" s="1">
-        <v>0.28272068916666698</v>
-      </c>
-      <c r="AA4" s="1">
-        <v>-1.5</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>5</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="AD4" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="AE4" s="1">
-        <v>5</v>
-      </c>
-      <c r="AF4" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F1:F3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="W1:AJ1"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AC2"/>
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:V1"/>
@@ -826,14 +700,12 @@
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W1:AJ1"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix excel handler for case
</commit_message>
<xml_diff>
--- a/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
+++ b/Simulator/Simulator/bin/Debug/temp/stats/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\TestSimulator\Simulator\Simulator\bin\Debug\temp\stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C7508A-0644-4BE1-B6AD-B47B23B4A079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB124FC7-B765-44F0-8308-5CEC465326C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13185" yWindow="765" windowWidth="16455" windowHeight="20625" xr2:uid="{8E2B3CB3-AB10-496A-9F08-311CA960E8CE}"/>
+    <workbookView xWindow="13185" yWindow="765" windowWidth="16455" windowHeight="20625" xr2:uid="{E96ECFE0-B987-4E47-B744-950EEF23D3CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="78">
   <si>
     <t>ФИО</t>
   </si>
@@ -80,6 +80,24 @@
     <t>П2</t>
   </si>
   <si>
+    <t>П3</t>
+  </si>
+  <si>
+    <t>П4</t>
+  </si>
+  <si>
+    <t>П5</t>
+  </si>
+  <si>
+    <t>П6</t>
+  </si>
+  <si>
+    <t>П7</t>
+  </si>
+  <si>
+    <t>П8</t>
+  </si>
+  <si>
     <t>Баллы, набранные за 1 попытку</t>
   </si>
   <si>
@@ -98,10 +116,160 @@
     <t>Этап 2</t>
   </si>
   <si>
-    <t>П4</t>
-  </si>
-  <si>
-    <t>П5</t>
+    <t>П10</t>
+  </si>
+  <si>
+    <t>П11</t>
+  </si>
+  <si>
+    <t>П12</t>
+  </si>
+  <si>
+    <t>П13</t>
+  </si>
+  <si>
+    <t>П14</t>
+  </si>
+  <si>
+    <t>П15</t>
+  </si>
+  <si>
+    <t>П16</t>
+  </si>
+  <si>
+    <t>П17</t>
+  </si>
+  <si>
+    <t>П18</t>
+  </si>
+  <si>
+    <t>П19</t>
+  </si>
+  <si>
+    <t>П20</t>
+  </si>
+  <si>
+    <t>П21</t>
+  </si>
+  <si>
+    <t>Этап 3</t>
+  </si>
+  <si>
+    <t>П23</t>
+  </si>
+  <si>
+    <t>П24</t>
+  </si>
+  <si>
+    <t>П25</t>
+  </si>
+  <si>
+    <t>П26</t>
+  </si>
+  <si>
+    <t>П27</t>
+  </si>
+  <si>
+    <t>Куляй Кирилл</t>
+  </si>
+  <si>
+    <t>3530404-10002</t>
+  </si>
+  <si>
+    <t>Максим Приймак</t>
+  </si>
+  <si>
+    <t>3530904-10002</t>
+  </si>
+  <si>
+    <t>Тимур Карама</t>
+  </si>
+  <si>
+    <t>1-2-3-4-8-</t>
+  </si>
+  <si>
+    <t>1-</t>
+  </si>
+  <si>
+    <t>1-3-4-</t>
+  </si>
+  <si>
+    <t>1-2-5-9-</t>
+  </si>
+  <si>
+    <t>4-</t>
+  </si>
+  <si>
+    <t>Сергей Шеремет</t>
+  </si>
+  <si>
+    <t>1-2-3-4-5-6-7-8-9-</t>
+  </si>
+  <si>
+    <t>1-2-3-4-5-6-7-</t>
+  </si>
+  <si>
+    <t>2-7-</t>
+  </si>
+  <si>
+    <t>1-2-3-4-5-</t>
+  </si>
+  <si>
+    <t>Глеб Жуков</t>
+  </si>
+  <si>
+    <t>2;3;5;6;</t>
+  </si>
+  <si>
+    <t>5;6;7;8;</t>
+  </si>
+  <si>
+    <t>3;</t>
+  </si>
+  <si>
+    <t>5;</t>
+  </si>
+  <si>
+    <t>1;</t>
+  </si>
+  <si>
+    <t>6;</t>
+  </si>
+  <si>
+    <t>2;3;4;</t>
+  </si>
+  <si>
+    <t>7;</t>
+  </si>
+  <si>
+    <t>9;</t>
+  </si>
+  <si>
+    <t>4;5;6;7;</t>
+  </si>
+  <si>
+    <t>8;</t>
+  </si>
+  <si>
+    <t>3;4;</t>
+  </si>
+  <si>
+    <t>5;6;7;</t>
+  </si>
+  <si>
+    <t>3;4;6;</t>
+  </si>
+  <si>
+    <t>3;4;5;</t>
+  </si>
+  <si>
+    <t>2;3;</t>
+  </si>
+  <si>
+    <t>2;</t>
+  </si>
+  <si>
+    <t>4;</t>
   </si>
 </sst>
 </file>
@@ -137,12 +305,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -458,8 +635,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F679A1BC-AC5E-4533-838D-9592A9E53D2B}">
-  <dimension ref="A1:AJ3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF83B1A3-0095-4CD7-B59E-3FD289574B55}">
+  <dimension ref="A1:EO8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A3"/>
@@ -470,7 +647,7 @@
     <col min="1" max="16384" width="15.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -511,9 +688,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
-      <c r="W1" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
@@ -527,8 +702,121 @@
       <c r="AH1" s="2"/>
       <c r="AI1" s="2"/>
       <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+      <c r="BF1" s="2"/>
+      <c r="BG1" s="2"/>
+      <c r="BH1" s="2"/>
+      <c r="BI1" s="2"/>
+      <c r="BJ1" s="2"/>
+      <c r="BK1" s="2"/>
+      <c r="BL1" s="2"/>
+      <c r="BM1" s="2"/>
+      <c r="BN1" s="2"/>
+      <c r="BO1" s="2"/>
+      <c r="BP1" s="2"/>
+      <c r="BQ1" s="2"/>
+      <c r="BR1" s="2"/>
+      <c r="BS1" s="2"/>
+      <c r="BT1" s="2"/>
+      <c r="BU1" s="2"/>
+      <c r="BV1" s="2"/>
+      <c r="BW1" s="2"/>
+      <c r="BX1" s="2"/>
+      <c r="BY1" s="2"/>
+      <c r="BZ1" s="2"/>
+      <c r="CA1" s="2"/>
+      <c r="CB1" s="2"/>
+      <c r="CC1" s="2"/>
+      <c r="CD1" s="2"/>
+      <c r="CE1" s="2"/>
+      <c r="CF1" s="2"/>
+      <c r="CG1" s="2"/>
+      <c r="CH1" s="2"/>
+      <c r="CI1" s="2"/>
+      <c r="CJ1" s="2"/>
+      <c r="CK1" s="2"/>
+      <c r="CL1" s="2"/>
+      <c r="CM1" s="2"/>
+      <c r="CN1" s="2"/>
+      <c r="CO1" s="2"/>
+      <c r="CP1" s="2"/>
+      <c r="CQ1" s="2"/>
+      <c r="CR1" s="2"/>
+      <c r="CS1" s="2"/>
+      <c r="CT1" s="2"/>
+      <c r="CU1" s="2"/>
+      <c r="CV1" s="2"/>
+      <c r="CW1" s="2"/>
+      <c r="CX1" s="2"/>
+      <c r="CY1" s="2"/>
+      <c r="CZ1" s="2"/>
+      <c r="DA1" s="2"/>
+      <c r="DB1" s="2"/>
+      <c r="DC1" s="2"/>
+      <c r="DD1" s="2"/>
+      <c r="DE1" s="2"/>
+      <c r="DF1" s="2"/>
+      <c r="DG1" s="2"/>
+      <c r="DH1" s="2"/>
+      <c r="DI1" s="2"/>
+      <c r="DJ1" s="2"/>
+      <c r="DK1" s="2"/>
+      <c r="DL1" s="2"/>
+      <c r="DM1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="DN1" s="2"/>
+      <c r="DO1" s="2"/>
+      <c r="DP1" s="2"/>
+      <c r="DQ1" s="2"/>
+      <c r="DR1" s="2"/>
+      <c r="DS1" s="2"/>
+      <c r="DT1" s="2"/>
+      <c r="DU1" s="2"/>
+      <c r="DV1" s="2"/>
+      <c r="DW1" s="2"/>
+      <c r="DX1" s="2"/>
+      <c r="DY1" s="2"/>
+      <c r="DZ1" s="2"/>
+      <c r="EA1" s="2"/>
+      <c r="EB1" s="2"/>
+      <c r="EC1" s="2"/>
+      <c r="ED1" s="2"/>
+      <c r="EE1" s="2"/>
+      <c r="EF1" s="2"/>
+      <c r="EG1" s="2"/>
+      <c r="EH1" s="2"/>
+      <c r="EI1" s="2"/>
+      <c r="EJ1" s="2"/>
+      <c r="EK1" s="2"/>
+      <c r="EL1" s="2"/>
+      <c r="EM1" s="2"/>
+      <c r="EN1" s="2"/>
+      <c r="EO1" s="2"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -547,54 +835,177 @@
         <v>11</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="T2" s="2"/>
-      <c r="U2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-      <c r="W2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="AC2" s="2"/>
-      <c r="AD2" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
-      <c r="AG2" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="AG2" s="2"/>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="AI2" s="2"/>
       <c r="AJ2" s="2"/>
+      <c r="AK2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="BD2" s="2"/>
+      <c r="BE2" s="2"/>
+      <c r="BF2" s="2"/>
+      <c r="BG2" s="2"/>
+      <c r="BH2" s="2"/>
+      <c r="BI2" s="2"/>
+      <c r="BJ2" s="2"/>
+      <c r="BK2" s="2"/>
+      <c r="BL2" s="2"/>
+      <c r="BM2" s="2"/>
+      <c r="BN2" s="2"/>
+      <c r="BO2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BP2" s="2"/>
+      <c r="BQ2" s="2"/>
+      <c r="BR2" s="2"/>
+      <c r="BS2" s="2"/>
+      <c r="BT2" s="2"/>
+      <c r="BU2" s="2"/>
+      <c r="BV2" s="2"/>
+      <c r="BW2" s="2"/>
+      <c r="BX2" s="2"/>
+      <c r="BY2" s="2"/>
+      <c r="BZ2" s="2"/>
+      <c r="CA2" s="2"/>
+      <c r="CB2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="CC2" s="2"/>
+      <c r="CD2" s="2"/>
+      <c r="CE2" s="2"/>
+      <c r="CF2" s="2"/>
+      <c r="CG2" s="2"/>
+      <c r="CH2" s="2"/>
+      <c r="CI2" s="2"/>
+      <c r="CJ2" s="2"/>
+      <c r="CK2" s="2"/>
+      <c r="CL2" s="2"/>
+      <c r="CM2" s="2"/>
+      <c r="CN2" s="2"/>
+      <c r="CO2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="CP2" s="2"/>
+      <c r="CQ2" s="2"/>
+      <c r="CR2" s="2"/>
+      <c r="CS2" s="2"/>
+      <c r="CT2" s="2"/>
+      <c r="CU2" s="2"/>
+      <c r="CV2" s="2"/>
+      <c r="CW2" s="2"/>
+      <c r="CX2" s="2"/>
+      <c r="CY2" s="2"/>
+      <c r="CZ2" s="2"/>
+      <c r="DA2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="DB2" s="2"/>
+      <c r="DC2" s="2"/>
+      <c r="DD2" s="2"/>
+      <c r="DE2" s="2"/>
+      <c r="DF2" s="2"/>
+      <c r="DG2" s="2"/>
+      <c r="DH2" s="2"/>
+      <c r="DI2" s="2"/>
+      <c r="DJ2" s="2"/>
+      <c r="DK2" s="2"/>
+      <c r="DL2" s="2"/>
+      <c r="DM2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="DN2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="DO2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="DP2" s="2"/>
+      <c r="DQ2" s="2"/>
+      <c r="DR2" s="2"/>
+      <c r="DS2" s="2"/>
+      <c r="DT2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="DU2" s="2"/>
+      <c r="DV2" s="2"/>
+      <c r="DW2" s="2"/>
+      <c r="DX2" s="2"/>
+      <c r="DY2" s="2"/>
+      <c r="DZ2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="EA2" s="2"/>
+      <c r="EB2" s="2"/>
+      <c r="EC2" s="2"/>
+      <c r="ED2" s="2"/>
+      <c r="EE2" s="2"/>
+      <c r="EF2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="EG2" s="2"/>
+      <c r="EH2" s="2"/>
+      <c r="EI2" s="2"/>
+      <c r="EJ2" s="2"/>
+      <c r="EK2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="EL2" s="2"/>
+      <c r="EM2" s="2"/>
+      <c r="EN2" s="2"/>
+      <c r="EO2" s="2"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -612,22 +1023,22 @@
         <v>13</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>12</v>
@@ -636,76 +1047,1095 @@
         <v>13</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="AF3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AJ3" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="AK3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BD3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BG3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BH3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BI3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BL3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BO3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BP3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BQ3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BR3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BS3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BT3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BU3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BV3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BW3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BX3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BY3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BZ3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CA3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="CB3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CC3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="CD3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="CE3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CF3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="CG3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="CH3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="CI3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="CJ3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="CK3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="CL3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CM3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="CN3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="CO3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CP3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="CQ3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="CR3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CS3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="CT3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="CU3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="CV3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="CW3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="CX3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="CY3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="DA3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="DB3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="DC3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="DD3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="DE3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="DF3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="DG3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="DH3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="DI3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="DJ3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="DK3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="DM3" s="2"/>
+      <c r="DN3" s="2"/>
+      <c r="DO3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="DP3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="DQ3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="DR3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DS3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="DT3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="DU3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="DV3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="DW3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="DX3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="DY3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="DZ3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="EA3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="EB3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="EC3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="ED3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="EE3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="EF3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="EG3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="EH3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="EI3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="EJ3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="EK3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="EL3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="EM3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="EN3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="EO3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:145" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1729203905</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45111.463101851848</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45111.440983796296</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM4" s="4">
+        <v>0</v>
+      </c>
+      <c r="DN4" s="4">
+        <v>0</v>
+      </c>
+      <c r="DY4" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:145" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1942717174</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="3">
+        <v>45110.833020833335</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM5" s="4">
+        <v>0</v>
+      </c>
+      <c r="DN5" s="4">
+        <v>0</v>
+      </c>
+      <c r="DY5" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:145" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1">
+        <v>301507971</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45110.771307870367</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>3.3686574074074075E-3</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.44199464166666702</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.12870805666666699</v>
+      </c>
+      <c r="M6" s="1">
+        <v>6.8029588333333293E-2</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.252257391666667</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0.52487950166666697</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0.10787421833333299</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>2.4418468899999999</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0.885281648333333</v>
+      </c>
+      <c r="S6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>3</v>
+      </c>
+      <c r="W6" s="1">
+        <v>6</v>
+      </c>
+      <c r="X6" s="1">
+        <v>-2</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>17</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BA6" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM6" s="4">
+        <v>0</v>
+      </c>
+      <c r="DN6" s="4">
+        <v>0</v>
+      </c>
+      <c r="DY6" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:145" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1">
+        <v>303363064</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45110.76525462963</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>9</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2.0453703703703701E-3</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.19764520499999999</v>
+      </c>
+      <c r="L7" s="1">
+        <v>4.5932486666666703E-2</v>
+      </c>
+      <c r="M7" s="1">
+        <v>7.7794133333333307E-2</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.23520043666666701</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.106433825</v>
+      </c>
+      <c r="P7" s="1">
+        <v>4.2732908333333298E-2</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>2.09613153166667</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.14346509166666699</v>
+      </c>
+      <c r="S7" s="1">
+        <v>3</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0</v>
+      </c>
+      <c r="V7" s="1">
+        <v>5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="X7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>-7</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>9</v>
+      </c>
+      <c r="AJ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AN7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AR7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA7" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM7" s="4">
+        <v>0</v>
+      </c>
+      <c r="DN7" s="4">
+        <v>0</v>
+      </c>
+      <c r="DY7" s="1">
+        <v>0</v>
+      </c>
+      <c r="EE7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:145" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1">
+        <v>438910696</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3">
+        <v>45111.595034722224</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45111.596631944441</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="H8" s="1">
+        <v>34</v>
+      </c>
+      <c r="I8" s="5">
+        <v>4.2942129629629624E-4</v>
+      </c>
+      <c r="J8" s="5">
+        <v>2.8200231481481479E-4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>7.0475334166666695E-2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>5.1003308333333303E-2</v>
+      </c>
+      <c r="M8" s="1">
+        <v>2.6315794999999999E-2</v>
+      </c>
+      <c r="N8" s="1">
+        <v>4.9347130000000003E-2</v>
+      </c>
+      <c r="O8" s="1">
+        <v>4.0787919999999998E-2</v>
+      </c>
+      <c r="P8" s="1">
+        <v>3.2600043333333301E-2</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0.19875780666666701</v>
+      </c>
+      <c r="R8" s="1">
+        <v>4.2933855E-2</v>
+      </c>
+      <c r="S8" s="1">
+        <v>3</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0</v>
+      </c>
+      <c r="V8" s="1">
+        <v>1</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>13</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AU8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AW8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA8" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="5">
+        <v>2.5798611111111112E-4</v>
+      </c>
+      <c r="BC8" s="1">
+        <v>3.8703363333333303E-2</v>
+      </c>
+      <c r="BD8" s="1">
+        <v>3.4312796666666701E-2</v>
+      </c>
+      <c r="BE8" s="1">
+        <v>1.3460966666666701E-2</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>3.9210476666666702E-2</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>4.1208864999999997E-2</v>
+      </c>
+      <c r="BH8" s="1">
+        <v>3.3558539999999998E-2</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>2.6483518333333299E-2</v>
+      </c>
+      <c r="BJ8" s="1">
+        <v>3.7569295000000003E-2</v>
+      </c>
+      <c r="BK8" s="1">
+        <v>3.6608708333333302E-2</v>
+      </c>
+      <c r="BL8" s="1">
+        <v>1.5219275000000001E-2</v>
+      </c>
+      <c r="BN8" s="1">
+        <v>5.5169553333333302E-2</v>
+      </c>
+      <c r="CA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB8" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC8" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="CD8" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="CE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="CG8" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH8" s="1">
+        <v>4</v>
+      </c>
+      <c r="CI8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="CJ8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="CK8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="CM8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CN8" s="1">
+        <v>17</v>
+      </c>
+      <c r="DA8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="DB8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="DC8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="DD8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="DE8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="DF8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="DG8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="DH8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="DI8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="DJ8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="DL8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="DM8" s="4">
+        <v>0</v>
+      </c>
+      <c r="DN8" s="5">
+        <v>7.8668981481481483E-5</v>
+      </c>
+      <c r="DO8" s="1">
+        <v>2.90523866666667E-2</v>
+      </c>
+      <c r="DP8" s="1">
+        <v>2.4402996666666701E-2</v>
+      </c>
+      <c r="DR8" s="1">
+        <v>3.8769908333333297E-2</v>
+      </c>
+      <c r="DS8" s="1">
+        <v>2.1056370000000001E-2</v>
+      </c>
+      <c r="DY8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="EA8" s="1">
+        <v>2</v>
+      </c>
+      <c r="EC8" s="1">
+        <v>1</v>
+      </c>
+      <c r="ED8" s="1">
+        <v>1</v>
+      </c>
+      <c r="EE8" s="1">
+        <v>4</v>
+      </c>
+      <c r="EK8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="EL8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="EN8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="EO8" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="W1:AJ1"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="AD2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:V1"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
+  <mergeCells count="32">
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
+    <mergeCell ref="G1:G3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:AZ1"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="S2:AA2"/>
+    <mergeCell ref="AB2:AJ2"/>
+    <mergeCell ref="AK2:AR2"/>
+    <mergeCell ref="AS2:AZ2"/>
+    <mergeCell ref="BA1:DL1"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="BC2:BN2"/>
+    <mergeCell ref="BO2:CA2"/>
+    <mergeCell ref="CB2:CN2"/>
+    <mergeCell ref="CO2:CZ2"/>
+    <mergeCell ref="DA2:DL2"/>
+    <mergeCell ref="DM1:EO1"/>
+    <mergeCell ref="DM2:DM3"/>
+    <mergeCell ref="DN2:DN3"/>
+    <mergeCell ref="DO2:DS2"/>
+    <mergeCell ref="DT2:DY2"/>
+    <mergeCell ref="DZ2:EE2"/>
+    <mergeCell ref="EF2:EJ2"/>
+    <mergeCell ref="EK2:EO2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>